<commit_message>
prueba de las 1010 am
</commit_message>
<xml_diff>
--- a/Backend/precios_colchones.xlsx
+++ b/Backend/precios_colchones.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flia aliamdri\OneDrive\Desktop\colchonespremium\Backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adr\Desktop\Colchonqn\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="350">
   <si>
     <t>Almohada Venecia 0.65 Inducol 1 UN</t>
   </si>
@@ -1070,28 +1070,10 @@
     <t>Mostrar</t>
   </si>
   <si>
-    <t>Imagen</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>si</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/NzjeCkw.jpeg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/pTv3BgX.jpeg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/Hvm9q5u.jpeg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/gK6TFQ1.jpeg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/fZ2rJGD.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1081,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1162,9 +1144,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1172,7 +1154,6 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda 2" xfId="2"/>
@@ -1456,20 +1437,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:E340"/>
+  <dimension ref="A1:D340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -1482,11 +1462,8 @@
       <c r="D1" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,13 +1474,10 @@
         <v>342</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1514,13 +1488,10 @@
         <v>342</v>
       </c>
       <c r="D3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1531,13 +1502,10 @@
         <v>342</v>
       </c>
       <c r="D4" t="s">
-        <v>350</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1548,10 +1516,10 @@
         <v>342</v>
       </c>
       <c r="D5" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1562,10 +1530,10 @@
         <v>342</v>
       </c>
       <c r="D6" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1576,10 +1544,10 @@
         <v>342</v>
       </c>
       <c r="D7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1590,10 +1558,10 @@
         <v>342</v>
       </c>
       <c r="D8" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1604,10 +1572,10 @@
         <v>342</v>
       </c>
       <c r="D9" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1618,10 +1586,10 @@
         <v>342</v>
       </c>
       <c r="D10" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1632,10 +1600,10 @@
         <v>342</v>
       </c>
       <c r="D11" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1646,10 +1614,10 @@
         <v>342</v>
       </c>
       <c r="D12" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1660,10 +1628,10 @@
         <v>342</v>
       </c>
       <c r="D13" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1674,10 +1642,10 @@
         <v>342</v>
       </c>
       <c r="D14" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1688,10 +1656,10 @@
         <v>342</v>
       </c>
       <c r="D15" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1702,7 +1670,7 @@
         <v>342</v>
       </c>
       <c r="D16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1716,7 +1684,7 @@
         <v>342</v>
       </c>
       <c r="D17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1730,7 +1698,7 @@
         <v>342</v>
       </c>
       <c r="D18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1744,7 +1712,7 @@
         <v>342</v>
       </c>
       <c r="D19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,7 +1726,7 @@
         <v>342</v>
       </c>
       <c r="D20" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1772,7 +1740,7 @@
         <v>342</v>
       </c>
       <c r="D21" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,7 +1754,7 @@
         <v>343</v>
       </c>
       <c r="D22" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1800,7 +1768,7 @@
         <v>344</v>
       </c>
       <c r="D23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1814,7 +1782,7 @@
         <v>344</v>
       </c>
       <c r="D24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1828,7 +1796,7 @@
         <v>344</v>
       </c>
       <c r="D25" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1842,7 +1810,7 @@
         <v>344</v>
       </c>
       <c r="D26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1856,7 +1824,7 @@
         <v>344</v>
       </c>
       <c r="D27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1870,7 +1838,7 @@
         <v>344</v>
       </c>
       <c r="D28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,7 +1852,7 @@
         <v>344</v>
       </c>
       <c r="D29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1898,7 +1866,7 @@
         <v>344</v>
       </c>
       <c r="D30" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,7 +1880,7 @@
         <v>344</v>
       </c>
       <c r="D31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,7 +1894,7 @@
         <v>344</v>
       </c>
       <c r="D32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1940,7 +1908,7 @@
         <v>344</v>
       </c>
       <c r="D33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1954,7 +1922,7 @@
         <v>344</v>
       </c>
       <c r="D34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1968,7 +1936,7 @@
         <v>344</v>
       </c>
       <c r="D35" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1982,7 +1950,7 @@
         <v>344</v>
       </c>
       <c r="D36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1996,7 +1964,7 @@
         <v>344</v>
       </c>
       <c r="D37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2010,7 +1978,7 @@
         <v>344</v>
       </c>
       <c r="D38" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2024,7 +1992,7 @@
         <v>344</v>
       </c>
       <c r="D39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2038,7 +2006,7 @@
         <v>344</v>
       </c>
       <c r="D40" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2052,7 +2020,7 @@
         <v>344</v>
       </c>
       <c r="D41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2066,7 +2034,7 @@
         <v>344</v>
       </c>
       <c r="D42" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2080,7 +2048,7 @@
         <v>344</v>
       </c>
       <c r="D43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2094,7 +2062,7 @@
         <v>344</v>
       </c>
       <c r="D44" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,7 +2076,7 @@
         <v>344</v>
       </c>
       <c r="D45" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2122,7 +2090,7 @@
         <v>344</v>
       </c>
       <c r="D46" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2136,7 +2104,7 @@
         <v>344</v>
       </c>
       <c r="D47" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2150,7 +2118,7 @@
         <v>344</v>
       </c>
       <c r="D48" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,7 +2132,7 @@
         <v>344</v>
       </c>
       <c r="D49" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2178,7 +2146,7 @@
         <v>344</v>
       </c>
       <c r="D50" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2192,7 +2160,7 @@
         <v>344</v>
       </c>
       <c r="D51" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2206,7 +2174,7 @@
         <v>344</v>
       </c>
       <c r="D52" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2220,7 +2188,7 @@
         <v>344</v>
       </c>
       <c r="D53" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2234,7 +2202,7 @@
         <v>344</v>
       </c>
       <c r="D54" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2248,7 +2216,7 @@
         <v>344</v>
       </c>
       <c r="D55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2262,7 +2230,7 @@
         <v>344</v>
       </c>
       <c r="D56" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2276,7 +2244,7 @@
         <v>344</v>
       </c>
       <c r="D57" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2290,7 +2258,7 @@
         <v>344</v>
       </c>
       <c r="D58" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2304,7 +2272,7 @@
         <v>344</v>
       </c>
       <c r="D59" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2318,7 +2286,7 @@
         <v>344</v>
       </c>
       <c r="D60" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2332,7 +2300,7 @@
         <v>344</v>
       </c>
       <c r="D61" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2346,7 +2314,7 @@
         <v>344</v>
       </c>
       <c r="D62" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2360,7 +2328,7 @@
         <v>344</v>
       </c>
       <c r="D63" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2374,7 +2342,7 @@
         <v>344</v>
       </c>
       <c r="D64" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2388,7 +2356,7 @@
         <v>344</v>
       </c>
       <c r="D65" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2402,7 +2370,7 @@
         <v>344</v>
       </c>
       <c r="D66" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2416,7 +2384,7 @@
         <v>344</v>
       </c>
       <c r="D67" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2430,7 +2398,7 @@
         <v>344</v>
       </c>
       <c r="D68" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2444,7 +2412,7 @@
         <v>344</v>
       </c>
       <c r="D69" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2458,7 +2426,7 @@
         <v>344</v>
       </c>
       <c r="D70" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2472,7 +2440,7 @@
         <v>344</v>
       </c>
       <c r="D71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2486,7 +2454,7 @@
         <v>344</v>
       </c>
       <c r="D72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2500,7 +2468,7 @@
         <v>344</v>
       </c>
       <c r="D73" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2514,7 +2482,7 @@
         <v>344</v>
       </c>
       <c r="D74" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2528,7 +2496,7 @@
         <v>344</v>
       </c>
       <c r="D75" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2542,7 +2510,7 @@
         <v>344</v>
       </c>
       <c r="D76" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2556,7 +2524,7 @@
         <v>344</v>
       </c>
       <c r="D77" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2570,7 +2538,7 @@
         <v>344</v>
       </c>
       <c r="D78" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2584,7 +2552,7 @@
         <v>344</v>
       </c>
       <c r="D79" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2598,7 +2566,7 @@
         <v>344</v>
       </c>
       <c r="D80" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2612,7 +2580,7 @@
         <v>344</v>
       </c>
       <c r="D81" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2626,7 +2594,7 @@
         <v>344</v>
       </c>
       <c r="D82" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2640,7 +2608,7 @@
         <v>344</v>
       </c>
       <c r="D83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2654,7 +2622,7 @@
         <v>344</v>
       </c>
       <c r="D84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2668,7 +2636,7 @@
         <v>344</v>
       </c>
       <c r="D85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2682,7 +2650,7 @@
         <v>344</v>
       </c>
       <c r="D86" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2696,7 +2664,7 @@
         <v>344</v>
       </c>
       <c r="D87" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2710,7 +2678,7 @@
         <v>344</v>
       </c>
       <c r="D88" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2724,7 +2692,7 @@
         <v>344</v>
       </c>
       <c r="D89" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2738,7 +2706,7 @@
         <v>344</v>
       </c>
       <c r="D90" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2752,7 +2720,7 @@
         <v>344</v>
       </c>
       <c r="D91" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2766,7 +2734,7 @@
         <v>344</v>
       </c>
       <c r="D92" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2780,7 +2748,7 @@
         <v>344</v>
       </c>
       <c r="D93" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2794,7 +2762,7 @@
         <v>344</v>
       </c>
       <c r="D94" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2808,7 +2776,7 @@
         <v>344</v>
       </c>
       <c r="D95" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2822,7 +2790,7 @@
         <v>344</v>
       </c>
       <c r="D96" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2836,7 +2804,7 @@
         <v>344</v>
       </c>
       <c r="D97" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2850,7 +2818,7 @@
         <v>344</v>
       </c>
       <c r="D98" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2864,7 +2832,7 @@
         <v>344</v>
       </c>
       <c r="D99" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2878,7 +2846,7 @@
         <v>344</v>
       </c>
       <c r="D100" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2892,7 +2860,7 @@
         <v>344</v>
       </c>
       <c r="D101" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2906,7 +2874,7 @@
         <v>344</v>
       </c>
       <c r="D102" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2920,7 +2888,7 @@
         <v>344</v>
       </c>
       <c r="D103" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2934,7 +2902,7 @@
         <v>344</v>
       </c>
       <c r="D104" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2948,7 +2916,7 @@
         <v>344</v>
       </c>
       <c r="D105" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2962,7 +2930,7 @@
         <v>344</v>
       </c>
       <c r="D106" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2976,7 +2944,7 @@
         <v>344</v>
       </c>
       <c r="D107" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2990,7 +2958,7 @@
         <v>344</v>
       </c>
       <c r="D108" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3004,7 +2972,7 @@
         <v>344</v>
       </c>
       <c r="D109" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3018,7 +2986,7 @@
         <v>344</v>
       </c>
       <c r="D110" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3032,7 +3000,7 @@
         <v>344</v>
       </c>
       <c r="D111" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -3046,7 +3014,7 @@
         <v>344</v>
       </c>
       <c r="D112" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3060,7 +3028,7 @@
         <v>344</v>
       </c>
       <c r="D113" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3074,7 +3042,7 @@
         <v>344</v>
       </c>
       <c r="D114" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3088,7 +3056,7 @@
         <v>344</v>
       </c>
       <c r="D115" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3102,7 +3070,7 @@
         <v>344</v>
       </c>
       <c r="D116" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3116,7 +3084,7 @@
         <v>344</v>
       </c>
       <c r="D117" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3130,7 +3098,7 @@
         <v>344</v>
       </c>
       <c r="D118" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3144,7 +3112,7 @@
         <v>344</v>
       </c>
       <c r="D119" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3158,7 +3126,7 @@
         <v>344</v>
       </c>
       <c r="D120" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -3172,7 +3140,7 @@
         <v>344</v>
       </c>
       <c r="D121" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3186,7 +3154,7 @@
         <v>344</v>
       </c>
       <c r="D122" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3200,7 +3168,7 @@
         <v>344</v>
       </c>
       <c r="D123" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3214,7 +3182,7 @@
         <v>344</v>
       </c>
       <c r="D124" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3228,7 +3196,7 @@
         <v>344</v>
       </c>
       <c r="D125" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3242,7 +3210,7 @@
         <v>344</v>
       </c>
       <c r="D126" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3256,7 +3224,7 @@
         <v>344</v>
       </c>
       <c r="D127" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3270,7 +3238,7 @@
         <v>344</v>
       </c>
       <c r="D128" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3284,7 +3252,7 @@
         <v>344</v>
       </c>
       <c r="D129" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3298,7 +3266,7 @@
         <v>344</v>
       </c>
       <c r="D130" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3312,7 +3280,7 @@
         <v>344</v>
       </c>
       <c r="D131" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,7 +3294,7 @@
         <v>344</v>
       </c>
       <c r="D132" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -3340,7 +3308,7 @@
         <v>344</v>
       </c>
       <c r="D133" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,7 +3322,7 @@
         <v>344</v>
       </c>
       <c r="D134" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3368,7 +3336,7 @@
         <v>344</v>
       </c>
       <c r="D135" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,7 +3350,7 @@
         <v>344</v>
       </c>
       <c r="D136" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,7 +3364,7 @@
         <v>344</v>
       </c>
       <c r="D137" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -3410,7 +3378,7 @@
         <v>344</v>
       </c>
       <c r="D138" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3424,7 +3392,7 @@
         <v>344</v>
       </c>
       <c r="D139" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3438,7 +3406,7 @@
         <v>344</v>
       </c>
       <c r="D140" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3452,7 +3420,7 @@
         <v>344</v>
       </c>
       <c r="D141" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3466,7 +3434,7 @@
         <v>344</v>
       </c>
       <c r="D142" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3480,7 +3448,7 @@
         <v>344</v>
       </c>
       <c r="D143" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -3494,7 +3462,7 @@
         <v>344</v>
       </c>
       <c r="D144" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3508,7 +3476,7 @@
         <v>344</v>
       </c>
       <c r="D145" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3522,7 +3490,7 @@
         <v>344</v>
       </c>
       <c r="D146" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -3536,7 +3504,7 @@
         <v>344</v>
       </c>
       <c r="D147" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3550,7 +3518,7 @@
         <v>344</v>
       </c>
       <c r="D148" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3564,7 +3532,7 @@
         <v>344</v>
       </c>
       <c r="D149" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -3578,7 +3546,7 @@
         <v>344</v>
       </c>
       <c r="D150" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3592,7 +3560,7 @@
         <v>344</v>
       </c>
       <c r="D151" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -3606,7 +3574,7 @@
         <v>344</v>
       </c>
       <c r="D152" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3620,7 +3588,7 @@
         <v>344</v>
       </c>
       <c r="D153" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3634,7 +3602,7 @@
         <v>344</v>
       </c>
       <c r="D154" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3648,7 +3616,7 @@
         <v>344</v>
       </c>
       <c r="D155" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -3662,7 +3630,7 @@
         <v>344</v>
       </c>
       <c r="D156" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -3676,7 +3644,7 @@
         <v>344</v>
       </c>
       <c r="D157" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3690,7 +3658,7 @@
         <v>344</v>
       </c>
       <c r="D158" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3704,7 +3672,7 @@
         <v>344</v>
       </c>
       <c r="D159" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3718,10 +3686,10 @@
         <v>344</v>
       </c>
       <c r="D160" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
@@ -3732,10 +3700,10 @@
         <v>344</v>
       </c>
       <c r="D161" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
@@ -3746,10 +3714,10 @@
         <v>344</v>
       </c>
       <c r="D162" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
@@ -3760,10 +3728,10 @@
         <v>344</v>
       </c>
       <c r="D163" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -3774,10 +3742,10 @@
         <v>344</v>
       </c>
       <c r="D164" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
@@ -3788,10 +3756,10 @@
         <v>344</v>
       </c>
       <c r="D165" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
@@ -3802,10 +3770,10 @@
         <v>344</v>
       </c>
       <c r="D166" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>165</v>
       </c>
@@ -3816,10 +3784,10 @@
         <v>344</v>
       </c>
       <c r="D167" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>166</v>
       </c>
@@ -3830,10 +3798,10 @@
         <v>344</v>
       </c>
       <c r="D168" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>167</v>
       </c>
@@ -3844,10 +3812,10 @@
         <v>344</v>
       </c>
       <c r="D169" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>168</v>
       </c>
@@ -3858,10 +3826,10 @@
         <v>344</v>
       </c>
       <c r="D170" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>169</v>
       </c>
@@ -3872,10 +3840,10 @@
         <v>344</v>
       </c>
       <c r="D171" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>170</v>
       </c>
@@ -3886,10 +3854,10 @@
         <v>344</v>
       </c>
       <c r="D172" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>171</v>
       </c>
@@ -3900,13 +3868,10 @@
         <v>344</v>
       </c>
       <c r="D173" t="s">
-        <v>350</v>
-      </c>
-      <c r="E173" s="7" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>172</v>
       </c>
@@ -3917,10 +3882,10 @@
         <v>344</v>
       </c>
       <c r="D174" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>173</v>
       </c>
@@ -3931,10 +3896,10 @@
         <v>344</v>
       </c>
       <c r="D175" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>174</v>
       </c>
@@ -3945,10 +3910,10 @@
         <v>344</v>
       </c>
       <c r="D176" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>175</v>
       </c>
@@ -3959,10 +3924,10 @@
         <v>344</v>
       </c>
       <c r="D177" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>176</v>
       </c>
@@ -3973,13 +3938,10 @@
         <v>344</v>
       </c>
       <c r="D178" t="s">
-        <v>350</v>
-      </c>
-      <c r="E178" s="7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>177</v>
       </c>
@@ -3990,10 +3952,10 @@
         <v>344</v>
       </c>
       <c r="D179" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>178</v>
       </c>
@@ -4004,10 +3966,10 @@
         <v>344</v>
       </c>
       <c r="D180" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>179</v>
       </c>
@@ -4018,10 +3980,10 @@
         <v>344</v>
       </c>
       <c r="D181" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>180</v>
       </c>
@@ -4032,10 +3994,10 @@
         <v>344</v>
       </c>
       <c r="D182" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>181</v>
       </c>
@@ -4046,13 +4008,10 @@
         <v>344</v>
       </c>
       <c r="D183" t="s">
-        <v>350</v>
-      </c>
-      <c r="E183" s="7" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>182</v>
       </c>
@@ -4063,10 +4022,10 @@
         <v>344</v>
       </c>
       <c r="D184" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>183</v>
       </c>
@@ -4077,10 +4036,10 @@
         <v>344</v>
       </c>
       <c r="D185" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>184</v>
       </c>
@@ -4091,10 +4050,10 @@
         <v>344</v>
       </c>
       <c r="D186" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>185</v>
       </c>
@@ -4105,10 +4064,10 @@
         <v>344</v>
       </c>
       <c r="D187" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>186</v>
       </c>
@@ -4119,10 +4078,10 @@
         <v>344</v>
       </c>
       <c r="D188" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>187</v>
       </c>
@@ -4133,10 +4092,10 @@
         <v>344</v>
       </c>
       <c r="D189" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>188</v>
       </c>
@@ -4147,10 +4106,10 @@
         <v>344</v>
       </c>
       <c r="D190" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>189</v>
       </c>
@@ -4161,10 +4120,10 @@
         <v>344</v>
       </c>
       <c r="D191" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>190</v>
       </c>
@@ -4175,10 +4134,10 @@
         <v>344</v>
       </c>
       <c r="D192" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>191</v>
       </c>
@@ -4189,10 +4148,10 @@
         <v>344</v>
       </c>
       <c r="D193" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>192</v>
       </c>
@@ -4203,10 +4162,10 @@
         <v>344</v>
       </c>
       <c r="D194" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>193</v>
       </c>
@@ -4217,10 +4176,10 @@
         <v>344</v>
       </c>
       <c r="D195" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>194</v>
       </c>
@@ -4231,10 +4190,10 @@
         <v>344</v>
       </c>
       <c r="D196" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>195</v>
       </c>
@@ -4245,10 +4204,10 @@
         <v>344</v>
       </c>
       <c r="D197" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>196</v>
       </c>
@@ -4259,10 +4218,10 @@
         <v>344</v>
       </c>
       <c r="D198" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>197</v>
       </c>
@@ -4273,13 +4232,10 @@
         <v>344</v>
       </c>
       <c r="D199" t="s">
-        <v>350</v>
-      </c>
-      <c r="E199" s="7" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>198</v>
       </c>
@@ -4290,10 +4246,10 @@
         <v>344</v>
       </c>
       <c r="D200" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>199</v>
       </c>
@@ -4304,10 +4260,10 @@
         <v>345</v>
       </c>
       <c r="D201" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>200</v>
       </c>
@@ -4318,10 +4274,10 @@
         <v>345</v>
       </c>
       <c r="D202" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>201</v>
       </c>
@@ -4332,10 +4288,10 @@
         <v>345</v>
       </c>
       <c r="D203" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>202</v>
       </c>
@@ -4346,10 +4302,10 @@
         <v>345</v>
       </c>
       <c r="D204" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>203</v>
       </c>
@@ -4360,10 +4316,10 @@
         <v>345</v>
       </c>
       <c r="D205" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>204</v>
       </c>
@@ -4374,10 +4330,10 @@
         <v>345</v>
       </c>
       <c r="D206" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>205</v>
       </c>
@@ -4388,10 +4344,10 @@
         <v>345</v>
       </c>
       <c r="D207" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>206</v>
       </c>
@@ -4402,7 +4358,7 @@
         <v>345</v>
       </c>
       <c r="D208" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4372,7 @@
         <v>345</v>
       </c>
       <c r="D209" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4430,7 +4386,7 @@
         <v>345</v>
       </c>
       <c r="D210" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4444,7 +4400,7 @@
         <v>345</v>
       </c>
       <c r="D211" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -4458,7 +4414,7 @@
         <v>345</v>
       </c>
       <c r="D212" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -4472,7 +4428,7 @@
         <v>344</v>
       </c>
       <c r="D213" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -4486,7 +4442,7 @@
         <v>344</v>
       </c>
       <c r="D214" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -4500,7 +4456,7 @@
         <v>344</v>
       </c>
       <c r="D215" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -4514,7 +4470,7 @@
         <v>344</v>
       </c>
       <c r="D216" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -4528,7 +4484,7 @@
         <v>344</v>
       </c>
       <c r="D217" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -4542,7 +4498,7 @@
         <v>344</v>
       </c>
       <c r="D218" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -4556,7 +4512,7 @@
         <v>344</v>
       </c>
       <c r="D219" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -4570,7 +4526,7 @@
         <v>344</v>
       </c>
       <c r="D220" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -4584,7 +4540,7 @@
         <v>344</v>
       </c>
       <c r="D221" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -4598,7 +4554,7 @@
         <v>344</v>
       </c>
       <c r="D222" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -4612,7 +4568,7 @@
         <v>344</v>
       </c>
       <c r="D223" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4582,7 @@
         <v>344</v>
       </c>
       <c r="D224" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -4640,7 +4596,7 @@
         <v>344</v>
       </c>
       <c r="D225" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -4654,7 +4610,7 @@
         <v>344</v>
       </c>
       <c r="D226" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -4668,7 +4624,7 @@
         <v>344</v>
       </c>
       <c r="D227" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -4682,7 +4638,7 @@
         <v>344</v>
       </c>
       <c r="D228" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -4696,7 +4652,7 @@
         <v>344</v>
       </c>
       <c r="D229" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -4710,7 +4666,7 @@
         <v>344</v>
       </c>
       <c r="D230" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -4724,7 +4680,7 @@
         <v>344</v>
       </c>
       <c r="D231" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -4738,7 +4694,7 @@
         <v>344</v>
       </c>
       <c r="D232" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -4752,7 +4708,7 @@
         <v>344</v>
       </c>
       <c r="D233" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -4766,7 +4722,7 @@
         <v>344</v>
       </c>
       <c r="D234" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -4780,7 +4736,7 @@
         <v>344</v>
       </c>
       <c r="D235" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -4794,7 +4750,7 @@
         <v>344</v>
       </c>
       <c r="D236" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -4808,7 +4764,7 @@
         <v>344</v>
       </c>
       <c r="D237" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -4822,7 +4778,7 @@
         <v>344</v>
       </c>
       <c r="D238" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4792,7 @@
         <v>344</v>
       </c>
       <c r="D239" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -4850,7 +4806,7 @@
         <v>344</v>
       </c>
       <c r="D240" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -4864,7 +4820,7 @@
         <v>344</v>
       </c>
       <c r="D241" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -4878,7 +4834,7 @@
         <v>344</v>
       </c>
       <c r="D242" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -4892,7 +4848,7 @@
         <v>344</v>
       </c>
       <c r="D243" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -4906,7 +4862,7 @@
         <v>344</v>
       </c>
       <c r="D244" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -4920,7 +4876,7 @@
         <v>344</v>
       </c>
       <c r="D245" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -4934,7 +4890,7 @@
         <v>344</v>
       </c>
       <c r="D246" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -4948,7 +4904,7 @@
         <v>344</v>
       </c>
       <c r="D247" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -4962,7 +4918,7 @@
         <v>344</v>
       </c>
       <c r="D248" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -4976,7 +4932,7 @@
         <v>344</v>
       </c>
       <c r="D249" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -4990,7 +4946,7 @@
         <v>344</v>
       </c>
       <c r="D250" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -5004,7 +4960,7 @@
         <v>344</v>
       </c>
       <c r="D251" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -5018,7 +4974,7 @@
         <v>344</v>
       </c>
       <c r="D252" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -5032,7 +4988,7 @@
         <v>344</v>
       </c>
       <c r="D253" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,7 +5002,7 @@
         <v>344</v>
       </c>
       <c r="D254" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -5060,7 +5016,7 @@
         <v>344</v>
       </c>
       <c r="D255" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -5074,7 +5030,7 @@
         <v>344</v>
       </c>
       <c r="D256" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -5088,7 +5044,7 @@
         <v>344</v>
       </c>
       <c r="D257" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -5102,7 +5058,7 @@
         <v>344</v>
       </c>
       <c r="D258" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -5116,7 +5072,7 @@
         <v>344</v>
       </c>
       <c r="D259" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -5130,7 +5086,7 @@
         <v>344</v>
       </c>
       <c r="D260" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -5144,7 +5100,7 @@
         <v>344</v>
       </c>
       <c r="D261" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -5158,7 +5114,7 @@
         <v>344</v>
       </c>
       <c r="D262" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -5172,7 +5128,7 @@
         <v>344</v>
       </c>
       <c r="D263" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
@@ -5186,7 +5142,7 @@
         <v>344</v>
       </c>
       <c r="D264" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
@@ -5200,7 +5156,7 @@
         <v>344</v>
       </c>
       <c r="D265" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -5214,7 +5170,7 @@
         <v>344</v>
       </c>
       <c r="D266" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
@@ -5228,7 +5184,7 @@
         <v>344</v>
       </c>
       <c r="D267" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -5242,7 +5198,7 @@
         <v>344</v>
       </c>
       <c r="D268" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -5256,7 +5212,7 @@
         <v>344</v>
       </c>
       <c r="D269" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -5270,7 +5226,7 @@
         <v>344</v>
       </c>
       <c r="D270" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -5284,7 +5240,7 @@
         <v>344</v>
       </c>
       <c r="D271" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -5298,7 +5254,7 @@
         <v>344</v>
       </c>
       <c r="D272" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -5312,7 +5268,7 @@
         <v>344</v>
       </c>
       <c r="D273" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -5326,7 +5282,7 @@
         <v>344</v>
       </c>
       <c r="D274" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -5340,7 +5296,7 @@
         <v>344</v>
       </c>
       <c r="D275" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -5354,7 +5310,7 @@
         <v>344</v>
       </c>
       <c r="D276" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -5368,7 +5324,7 @@
         <v>344</v>
       </c>
       <c r="D277" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
@@ -5382,7 +5338,7 @@
         <v>344</v>
       </c>
       <c r="D278" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -5396,7 +5352,7 @@
         <v>344</v>
       </c>
       <c r="D279" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -5410,7 +5366,7 @@
         <v>344</v>
       </c>
       <c r="D280" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -5424,7 +5380,7 @@
         <v>344</v>
       </c>
       <c r="D281" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -5438,7 +5394,7 @@
         <v>344</v>
       </c>
       <c r="D282" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -5452,7 +5408,7 @@
         <v>345</v>
       </c>
       <c r="D283" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -5466,7 +5422,7 @@
         <v>345</v>
       </c>
       <c r="D284" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
@@ -5480,7 +5436,7 @@
         <v>346</v>
       </c>
       <c r="D285" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -5494,7 +5450,7 @@
         <v>346</v>
       </c>
       <c r="D286" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -5508,7 +5464,7 @@
         <v>346</v>
       </c>
       <c r="D287" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
@@ -5522,7 +5478,7 @@
         <v>346</v>
       </c>
       <c r="D288" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -5536,7 +5492,7 @@
         <v>346</v>
       </c>
       <c r="D289" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -5550,7 +5506,7 @@
         <v>346</v>
       </c>
       <c r="D290" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -5564,7 +5520,7 @@
         <v>346</v>
       </c>
       <c r="D291" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -5578,7 +5534,7 @@
         <v>346</v>
       </c>
       <c r="D292" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -5592,7 +5548,7 @@
         <v>346</v>
       </c>
       <c r="D293" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
@@ -5606,7 +5562,7 @@
         <v>346</v>
       </c>
       <c r="D294" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -5620,7 +5576,7 @@
         <v>346</v>
       </c>
       <c r="D295" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
@@ -5634,7 +5590,7 @@
         <v>346</v>
       </c>
       <c r="D296" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.25">
@@ -5648,7 +5604,7 @@
         <v>346</v>
       </c>
       <c r="D297" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -5662,7 +5618,7 @@
         <v>346</v>
       </c>
       <c r="D298" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -5676,7 +5632,7 @@
         <v>346</v>
       </c>
       <c r="D299" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -5690,7 +5646,7 @@
         <v>346</v>
       </c>
       <c r="D300" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -5704,7 +5660,7 @@
         <v>346</v>
       </c>
       <c r="D301" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
@@ -5718,7 +5674,7 @@
         <v>346</v>
       </c>
       <c r="D302" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -5732,7 +5688,7 @@
         <v>346</v>
       </c>
       <c r="D303" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
@@ -5746,7 +5702,7 @@
         <v>346</v>
       </c>
       <c r="D304" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
@@ -5760,7 +5716,7 @@
         <v>346</v>
       </c>
       <c r="D305" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -5774,7 +5730,7 @@
         <v>346</v>
       </c>
       <c r="D306" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -5788,7 +5744,7 @@
         <v>346</v>
       </c>
       <c r="D307" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -5802,7 +5758,7 @@
         <v>346</v>
       </c>
       <c r="D308" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -5816,7 +5772,7 @@
         <v>346</v>
       </c>
       <c r="D309" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -5830,7 +5786,7 @@
         <v>346</v>
       </c>
       <c r="D310" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -5844,7 +5800,7 @@
         <v>346</v>
       </c>
       <c r="D311" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -5858,7 +5814,7 @@
         <v>346</v>
       </c>
       <c r="D312" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -5872,7 +5828,7 @@
         <v>346</v>
       </c>
       <c r="D313" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
@@ -5886,7 +5842,7 @@
         <v>346</v>
       </c>
       <c r="D314" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -5900,7 +5856,7 @@
         <v>346</v>
       </c>
       <c r="D315" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
@@ -5914,7 +5870,7 @@
         <v>346</v>
       </c>
       <c r="D316" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -5928,7 +5884,7 @@
         <v>346</v>
       </c>
       <c r="D317" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -5942,7 +5898,7 @@
         <v>346</v>
       </c>
       <c r="D318" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -5956,7 +5912,7 @@
         <v>346</v>
       </c>
       <c r="D319" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -5970,7 +5926,7 @@
         <v>346</v>
       </c>
       <c r="D320" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -5984,7 +5940,7 @@
         <v>346</v>
       </c>
       <c r="D321" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
@@ -5998,7 +5954,7 @@
         <v>346</v>
       </c>
       <c r="D322" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
@@ -6012,7 +5968,7 @@
         <v>346</v>
       </c>
       <c r="D323" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -6026,7 +5982,7 @@
         <v>346</v>
       </c>
       <c r="D324" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -6040,7 +5996,7 @@
         <v>346</v>
       </c>
       <c r="D325" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -6054,7 +6010,7 @@
         <v>346</v>
       </c>
       <c r="D326" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -6068,7 +6024,7 @@
         <v>346</v>
       </c>
       <c r="D327" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -6082,7 +6038,7 @@
         <v>346</v>
       </c>
       <c r="D328" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -6096,7 +6052,7 @@
         <v>346</v>
       </c>
       <c r="D329" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -6110,7 +6066,7 @@
         <v>346</v>
       </c>
       <c r="D330" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -6124,7 +6080,7 @@
         <v>346</v>
       </c>
       <c r="D331" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
@@ -6138,7 +6094,7 @@
         <v>346</v>
       </c>
       <c r="D332" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -6152,7 +6108,7 @@
         <v>346</v>
       </c>
       <c r="D333" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -6166,7 +6122,7 @@
         <v>346</v>
       </c>
       <c r="D334" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -6180,7 +6136,7 @@
         <v>346</v>
       </c>
       <c r="D335" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -6194,7 +6150,7 @@
         <v>346</v>
       </c>
       <c r="D336" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -6208,7 +6164,7 @@
         <v>346</v>
       </c>
       <c r="D337" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6222,7 +6178,7 @@
         <v>346</v>
       </c>
       <c r="D338" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -6236,7 +6192,7 @@
         <v>346</v>
       </c>
       <c r="D339" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -6250,7 +6206,7 @@
         <v>346</v>
       </c>
       <c r="D340" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>